<commit_message>
Cambios en algunos datos y nombres
</commit_message>
<xml_diff>
--- a/Analisis/Metpro_TransporteDavid.xlsx
+++ b/Analisis/Metpro_TransporteDavid.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan Kelly\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan Kelly\Downloads\EasyHotBus\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93141B5-983D-4299-9D08-0E811DB0ED36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8649DA73-1B87-4844-9041-EA3F8C7E7FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada" sheetId="1" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>Se proporciona un Switch en el cual se proporcionara las siguientes opciones: - Información General por Bus -Mantenimientos por Bus -Ingreso por Bus(opción para imprimir un archivo con los datos regitrados)</t>
   </si>
   <si>
-    <t>Buses</t>
-  </si>
-  <si>
     <t>Sentido</t>
   </si>
   <si>
@@ -224,13 +221,16 @@
     <t>Vernon Dávila     Apodo: El Pekka</t>
   </si>
   <si>
-    <t>Aidan Kelly                    Apodo: El 4 ojos</t>
-  </si>
-  <si>
     <t>Bayardo López Apodo: El favorito de Duran</t>
   </si>
   <si>
     <t>Nombre: Easy Hot Bus</t>
+  </si>
+  <si>
+    <t>Gerencia</t>
+  </si>
+  <si>
+    <t>Aidan Kelly                    Apodo: El Lider</t>
   </si>
 </sst>
 </file>
@@ -510,33 +510,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -570,6 +543,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -579,11 +561,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -868,8 +868,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:J1048574"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17353" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -888,24 +888,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="40"/>
+      <c r="A1" s="29"/>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="40"/>
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
@@ -949,7 +949,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -968,7 +968,7 @@
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -987,7 +987,7 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1006,7 +1006,7 @@
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1025,7 +1025,7 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1044,7 +1044,7 @@
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1063,7 +1063,7 @@
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="15" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1082,8 +1082,8 @@
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="28" t="s">
-        <v>53</v>
+      <c r="B12" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>5</v>
@@ -1101,8 +1101,8 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="33" t="s">
-        <v>54</v>
+      <c r="B13" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>6</v>
@@ -1119,8 +1119,8 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="33" t="s">
-        <v>55</v>
+      <c r="B14" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>6</v>
@@ -1138,8 +1138,8 @@
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="33" t="s">
-        <v>56</v>
+      <c r="B15" s="24" t="s">
+        <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>6</v>
@@ -1157,7 +1157,7 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1176,7 +1176,7 @@
       <c r="J16" s="6"/>
     </row>
     <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1195,7 +1195,7 @@
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="24" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1214,7 +1214,7 @@
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1233,7 +1233,7 @@
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1252,7 +1252,7 @@
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="24" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1271,7 +1271,7 @@
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="24" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1290,7 +1290,7 @@
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="24" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1364,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,11 +1377,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
@@ -1404,85 +1404,85 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="32" t="s">
+      <c r="B4" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="32" t="s">
-        <v>57</v>
+      <c r="D4" s="23" t="s">
+        <v>56</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="26" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="31"/>
+    </row>
+    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="31"/>
+    </row>
+    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="37"/>
-    </row>
-    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="37"/>
-    </row>
-    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="38"/>
-    </row>
-    <row r="10" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -1553,7 +1553,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D12"/>
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,12 +1565,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1583,46 +1583,46 @@
         <v>23</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="36"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="36"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Se realizaron cambios tras la primera revisión
</commit_message>
<xml_diff>
--- a/Analisis/Metpro_TransporteDavid.xlsx
+++ b/Analisis/Metpro_TransporteDavid.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan Kelly\Downloads\EasyHotBus\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan Kelly\Desktop\EasyHotBus\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8649DA73-1B87-4844-9041-EA3F8C7E7FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE90AF3-F194-4973-A1ED-C3D704319D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
   <si>
     <t>Identificador</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Se proporciona los horarios de los buses y en que sentido de viaje van ya sea Nagarote Managua o al Contrario</t>
   </si>
   <si>
-    <t>Encargado</t>
-  </si>
-  <si>
     <t>Usuario</t>
   </si>
   <si>
@@ -206,38 +203,26 @@
     <t>Ganancia Final</t>
   </si>
   <si>
-    <t>Ganancia Diaria: VentasTotal - Egreso total Ganancia mensual= Ganancia Diaria *30         Ganacia Final = Ganancia Mensual - Mantenimiento</t>
-  </si>
-  <si>
     <t>Mostrar Usuario</t>
   </si>
   <si>
     <t>Se muestra al Usuario por medio del id</t>
   </si>
   <si>
-    <t>Hanssell Llanes     Apodo: El Diablo</t>
-  </si>
-  <si>
-    <t>Vernon Dávila     Apodo: El Pekka</t>
-  </si>
-  <si>
-    <t>Bayardo López Apodo: El favorito de Duran</t>
-  </si>
-  <si>
     <t>Nombre: Easy Hot Bus</t>
   </si>
   <si>
     <t>Gerencia</t>
   </si>
   <si>
-    <t>Aidan Kelly                    Apodo: El Lider</t>
+    <t>Global</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +245,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -303,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -438,48 +430,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -552,15 +507,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -584,6 +530,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -868,8 +827,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:J1048574"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17353" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -890,7 +849,7 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="29"/>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -958,7 +917,9 @@
       <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F5" s="11">
         <v>0</v>
       </c>
@@ -977,7 +938,9 @@
       <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F6" s="11">
         <v>0</v>
       </c>
@@ -996,7 +959,9 @@
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F7" s="11">
         <v>0</v>
       </c>
@@ -1015,7 +980,9 @@
       <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F8" s="10">
         <v>0</v>
       </c>
@@ -1034,7 +1001,9 @@
       <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F9" s="10">
         <v>0</v>
       </c>
@@ -1053,7 +1022,9 @@
       <c r="D10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F10" s="10">
         <v>0</v>
       </c>
@@ -1064,7 +1035,7 @@
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>5</v>
@@ -1072,7 +1043,9 @@
       <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F11" s="10">
         <v>0</v>
       </c>
@@ -1083,7 +1056,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>5</v>
@@ -1091,7 +1064,9 @@
       <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
@@ -1102,13 +1077,16 @@
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
@@ -1120,7 +1098,7 @@
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>6</v>
@@ -1128,7 +1106,9 @@
       <c r="D14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
@@ -1139,7 +1119,7 @@
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>6</v>
@@ -1147,7 +1127,9 @@
       <c r="D15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F15" s="10">
         <v>0</v>
       </c>
@@ -1166,7 +1148,9 @@
       <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
@@ -1185,7 +1169,9 @@
       <c r="D17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
@@ -1204,7 +1190,9 @@
       <c r="D18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F18" s="10">
         <v>0</v>
       </c>
@@ -1223,7 +1211,9 @@
       <c r="D19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F19" s="10">
         <v>0</v>
       </c>
@@ -1242,7 +1232,9 @@
       <c r="D20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F20" s="10">
         <v>0</v>
       </c>
@@ -1261,7 +1253,9 @@
       <c r="D21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F21" s="10">
         <v>0</v>
       </c>
@@ -1280,7 +1274,9 @@
       <c r="D22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="6"/>
+      <c r="E22" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F22" s="10">
         <v>0</v>
       </c>
@@ -1299,8 +1295,10 @@
       <c r="D23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="10">
+      <c r="E23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="42">
         <v>0</v>
       </c>
       <c r="G23" s="6"/>
@@ -1364,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1385,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1399,23 +1397,17 @@
       <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="E3" s="41"/>
     </row>
     <row r="4" spans="2:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>64</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
@@ -1425,119 +1417,113 @@
         <v>39</v>
       </c>
       <c r="D5" s="12"/>
-      <c r="E5" s="13" t="s">
-        <v>60</v>
-      </c>
+      <c r="E5" s="38"/>
     </row>
     <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="12"/>
-      <c r="E6" s="30" t="s">
-        <v>59</v>
-      </c>
+      <c r="E6" s="39"/>
     </row>
     <row r="7" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="31"/>
+      <c r="E7" s="39"/>
     </row>
     <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="31"/>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" s="13"/>
-      <c r="E9" s="32"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>61</v>
-      </c>
+      <c r="E10" s="38"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="E12" s="40"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="E13" s="40"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="E14" s="40"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="E16" s="40"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="E17" s="40"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="E18" s="40"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="E19" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1545,6 +1531,7 @@
     <mergeCell ref="E6:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1552,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,46 +1570,46 @@
         <v>23</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="37"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="33"/>
-      <c r="D4" s="34"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="35"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="35"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="35"/>
-      <c r="D8" s="36"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="35"/>
-      <c r="D10" s="36"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="35"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>